<commit_message>
add field-level validation and error messages
</commit_message>
<xml_diff>
--- a/src/data/Safety AD Data RCT small.xlsx
+++ b/src/data/Safety AD Data RCT small.xlsx
@@ -373,10 +373,10 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="H2 G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.84"/>
@@ -1210,10 +1210,10 @@
   <dimension ref="A1:H116"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="H2 G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.83"/>
@@ -4256,10 +4256,10 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.33"/>
   </cols>
@@ -4290,7 +4290,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>23807</v>
       </c>
@@ -4316,7 +4316,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>23807</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>33766</v>
       </c>

</xml_diff>

<commit_message>
validate that arm sheets have at least 2 unique study_id values
</commit_message>
<xml_diff>
--- a/src/data/Safety AD Data RCT small.xlsx
+++ b/src/data/Safety AD Data RCT small.xlsx
@@ -373,10 +373,10 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="H2 G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.84"/>
@@ -1209,11 +1209,11 @@
   </sheetPr>
   <dimension ref="A1:H116"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="H2 G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A160" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.83"/>
@@ -4256,10 +4256,10 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.33"/>
   </cols>

</xml_diff>

<commit_message>
strip column name spaces, add hdeader, reset file input contents on reset
</commit_message>
<xml_diff>
--- a/src/data/Safety AD Data RCT small.xlsx
+++ b/src/data/Safety AD Data RCT small.xlsx
@@ -376,7 +376,7 @@
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.84"/>
@@ -1213,7 +1213,7 @@
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.83"/>
@@ -4256,15 +4256,15 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.33"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>

</xml_diff>